<commit_message>
Check-in revised spreadsheet of components & prices
</commit_message>
<xml_diff>
--- a/doc/components.xlsx
+++ b/doc/components.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="468" windowWidth="15984" windowHeight="5232"/>
+    <workbookView xWindow="3380" yWindow="540" windowWidth="25040" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>Component List for REA/Canister System</t>
   </si>
@@ -34,30 +38,18 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>Mnfctr, if diff.</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Price ea.</t>
-  </si>
-  <si>
-    <t>Ext. price</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>Sonic anemometer</t>
   </si>
   <si>
-    <t>Gill (?)</t>
-  </si>
-  <si>
     <t>Data logger</t>
   </si>
   <si>
@@ -112,9 +104,6 @@
     <t>SS-10L-12V</t>
   </si>
   <si>
-    <t>L1 L2</t>
-  </si>
-  <si>
     <t>price is from MorningStar U.S. list prices</t>
   </si>
   <si>
@@ -220,21 +209,28 @@
     <t>Total cost</t>
   </si>
   <si>
-    <t>order today</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>81000VRE</t>
+  </si>
+  <si>
+    <t>Est. Price (ea)</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Manufactuer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0;[Red]&quot;-&quot;[$$-409]#,##0"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +267,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -289,7 +299,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -299,8 +309,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -318,20 +330,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
@@ -625,47 +640,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="18.296875" customWidth="1"/>
-    <col min="3" max="3" width="4.09765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.796875" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" customWidth="1"/>
-    <col min="7" max="7" width="4" customWidth="1"/>
-    <col min="8" max="8" width="6.796875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="7.3984375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="29.09765625" customWidth="1"/>
-    <col min="11" max="1025" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="1024" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" ht="17">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
       <c r="J3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="6" customFormat="1">
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>5</v>
@@ -673,558 +690,531 @@
       <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4">
+      <c r="G5" s="12">
         <v>3500</v>
       </c>
-      <c r="I5" s="5">
+      <c r="H5" s="12">
         <v>3500</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="12">
+        <v>3063</v>
+      </c>
+      <c r="H6" s="12">
+        <v>3063</v>
+      </c>
+      <c r="J6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="4">
-        <v>3063</v>
-      </c>
-      <c r="I6" s="5">
-        <v>3063</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="12">
+        <v>336</v>
+      </c>
+      <c r="H7" s="12">
+        <v>336</v>
+      </c>
+      <c r="J7" t="s">
         <v>16</v>
-      </c>
-      <c r="H7" s="11">
-        <v>336</v>
-      </c>
-      <c r="I7" s="5">
-        <v>336</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
         <v>2</v>
       </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="12">
+        <v>86</v>
+      </c>
+      <c r="H8" s="12">
+        <v>172</v>
+      </c>
+      <c r="J8" t="s">
         <v>16</v>
-      </c>
-      <c r="H8" s="11">
-        <v>86</v>
-      </c>
-      <c r="I8" s="5">
-        <v>172</v>
-      </c>
-      <c r="J8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
         <v>2</v>
       </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4">
+        <v>22</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="12">
         <v>699</v>
       </c>
-      <c r="I9" s="5">
+      <c r="H9" s="12">
         <v>1398</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12">
+        <v>75</v>
+      </c>
+      <c r="H10" s="12">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="12">
+        <v>104</v>
+      </c>
+      <c r="H11" s="12">
+        <v>416</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="4">
-        <v>75</v>
-      </c>
-      <c r="I10" s="5">
-        <v>75</v>
-      </c>
-      <c r="J10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="12">
+        <v>543</v>
+      </c>
+      <c r="H12" s="12">
+        <v>543</v>
+      </c>
+      <c r="J12" t="s">
         <v>16</v>
-      </c>
-      <c r="H11" s="4">
-        <v>104</v>
-      </c>
-      <c r="I11" s="5">
-        <v>416</v>
-      </c>
-      <c r="J11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="4">
-        <v>543</v>
-      </c>
-      <c r="I12" s="5">
-        <v>543</v>
-      </c>
-      <c r="J12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="12">
         <v>852</v>
       </c>
-      <c r="I13" s="5">
+      <c r="H13" s="12">
         <v>852</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2">
         <v>1</v>
       </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="12">
+        <v>643</v>
+      </c>
+      <c r="H14" s="12">
+        <v>643</v>
+      </c>
+      <c r="J14" t="s">
         <v>16</v>
-      </c>
-      <c r="H14" s="4">
-        <v>643</v>
-      </c>
-      <c r="I14" s="5">
-        <v>643</v>
-      </c>
-      <c r="J14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="2">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="11">
+        <v>44</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="12">
         <v>197</v>
       </c>
-      <c r="I15" s="5">
+      <c r="H15" s="12">
         <v>197</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="12">
+        <v>235</v>
+      </c>
+      <c r="H16" s="12">
+        <v>470</v>
+      </c>
+      <c r="J16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="12">
+        <v>13</v>
+      </c>
+      <c r="H17" s="12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="2">
+      <c r="B18" s="2">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="12">
+        <v>250</v>
+      </c>
+      <c r="H18" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
         <v>52</v>
       </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="4">
-        <v>235</v>
-      </c>
-      <c r="I16" s="5">
-        <v>470</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="12">
+        <v>150</v>
+      </c>
+      <c r="H19" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>400</v>
+      </c>
+      <c r="H20" s="12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="2">
+      <c r="B21" s="2">
+        <v>6</v>
+      </c>
+      <c r="G21" s="12">
+        <v>500</v>
+      </c>
+      <c r="H21" s="12">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22"/>
+      <c r="G22" s="12">
+        <v>200</v>
+      </c>
+      <c r="H22" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="12">
+        <v>165</v>
+      </c>
+      <c r="H23" s="12">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="11">
-        <v>13</v>
-      </c>
-      <c r="I17" s="5">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="2">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4">
-        <v>250</v>
-      </c>
-      <c r="I18" s="5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="B19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4">
-        <v>150</v>
-      </c>
-      <c r="I19" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4">
-        <v>400</v>
-      </c>
-      <c r="I20" s="5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6</v>
-      </c>
-      <c r="H21" s="4">
-        <v>500</v>
-      </c>
-      <c r="I21" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22"/>
-      <c r="H22" s="4">
-        <v>200</v>
-      </c>
-      <c r="I22" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="B23" s="12" t="s">
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="G26" s="9"/>
+      <c r="H26"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="H31" s="5">
+        <v>16256</v>
+      </c>
+      <c r="I31" t="s">
         <v>61</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="11">
-        <v>165</v>
-      </c>
-      <c r="I23" s="5">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="B24" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="B25" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="2">
-        <v>2</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="H26" s="11"/>
-      <c r="I26"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="I31" s="5">
-        <v>16256</v>
-      </c>
-      <c r="J31" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1"/>
-    <hyperlink ref="G7" r:id="rId2"/>
-    <hyperlink ref="G8" r:id="rId3"/>
-    <hyperlink ref="G9" r:id="rId4"/>
-    <hyperlink ref="G11" r:id="rId5"/>
-    <hyperlink ref="G12" r:id="rId6"/>
-    <hyperlink ref="G13" r:id="rId7"/>
-    <hyperlink ref="G14" r:id="rId8"/>
-    <hyperlink ref="G15" r:id="rId9"/>
-    <hyperlink ref="G16" r:id="rId10"/>
-    <hyperlink ref="G17" r:id="rId11"/>
-    <hyperlink ref="G23" r:id="rId12"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
+    <hyperlink ref="F9" r:id="rId4"/>
+    <hyperlink ref="F11" r:id="rId5"/>
+    <hyperlink ref="F12" r:id="rId6"/>
+    <hyperlink ref="F13" r:id="rId7"/>
+    <hyperlink ref="F14" r:id="rId8"/>
+    <hyperlink ref="F15" r:id="rId9"/>
+    <hyperlink ref="F16" r:id="rId10"/>
+    <hyperlink ref="F17" r:id="rId11"/>
+    <hyperlink ref="F23" r:id="rId12"/>
+    <hyperlink ref="F5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39410000000000001" bottom="0.39410000000000001" header="0" footer="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0" right="0" top="0.39410000000000001" bottom="0.39410000000000001" header="0" footer="0"/>
@@ -1232,18 +1222,23 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0" right="0" top="0.39410000000000001" bottom="0.39410000000000001" header="0" footer="0"/>
@@ -1251,5 +1246,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add to components: relay & cover for pump control
</commit_message>
<xml_diff>
--- a/doc/components.xlsx
+++ b/doc/components.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="136">
   <si>
     <t>Component List for REA/Canister System</t>
   </si>
@@ -296,13 +296,37 @@
     <t>NPK09DC</t>
   </si>
   <si>
+    <t>Relay, 5-60Vdc output, 0-5Vdc logic</t>
+  </si>
+  <si>
+    <t>Opto22</t>
+  </si>
+  <si>
+    <t>ODC5</t>
+  </si>
+  <si>
+    <t>For valve control</t>
+  </si>
+  <si>
+    <t>http://opto22.com/site/pr_details.aspx?cid=7&amp;item=ODC5 </t>
+  </si>
+  <si>
     <t>Relay mounting board</t>
   </si>
   <si>
-    <t>Opto22</t>
-  </si>
-  <si>
     <t>PB4R</t>
+  </si>
+  <si>
+    <t>Relay, solid state, 5-60Vdc output, 0-5Vdc logic</t>
+  </si>
+  <si>
+    <t>Crydom</t>
+  </si>
+  <si>
+    <t>For pump on/off</t>
+  </si>
+  <si>
+    <t>Relay, solid state, cover</t>
   </si>
   <si>
     <t>Solar array battery bank package</t>
@@ -626,17 +650,17 @@
     <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.2455357142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.1294642857143"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.35267857142857"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.4955357142857"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4955357142857"/>
@@ -671,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="n">
-        <f aca="false">SUM(F5:F1001)</f>
+        <f aca="false">SUM(F5:F1004)</f>
         <v>19617.58</v>
       </c>
       <c r="G2" s="8"/>
@@ -1445,12 +1469,12 @@
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>94</v>
@@ -1459,113 +1483,106 @@
         <v>95</v>
       </c>
       <c r="E34" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="G34" s="12" t="n">
+        <v>40358</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="1" t="n">
         <v>45</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <f aca="false">E34*B34</f>
-        <v>45</v>
-      </c>
-      <c r="G34" s="12" t="n">
-        <v>40355</v>
-      </c>
-      <c r="H34" s="0"/>
-      <c r="I34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>1898531</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>1543</v>
       </c>
       <c r="F35" s="1" t="n">
         <f aca="false">E35*B35</f>
-        <v>1543</v>
+        <v>45</v>
       </c>
       <c r="G35" s="12" t="n">
-        <v>40358</v>
+        <v>40355</v>
       </c>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1" t="n">
         <f aca="false">E36*B36</f>
-        <v>75</v>
-      </c>
-      <c r="G36" s="0"/>
-      <c r="H36" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="12" t="n">
+        <v>40358</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="I36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
-        <v>101</v>
+      <c r="A37" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" s="1" t="n">
-        <f aca="false">E37*B37</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="0"/>
-      <c r="H37" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="G37" s="12"/>
       <c r="I37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>102</v>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>1898531</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>685</v>
+        <v>1543</v>
       </c>
       <c r="F38" s="1" t="n">
         <f aca="false">E38*B38</f>
-        <v>685</v>
-      </c>
-      <c r="G38" s="0"/>
+        <v>1543</v>
+      </c>
+      <c r="G38" s="12" t="n">
+        <v>40358</v>
+      </c>
       <c r="H38" s="0"/>
-      <c r="I38" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>106</v>
       </c>
@@ -1579,184 +1596,214 @@
         <v>108</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="F39" s="1" t="n">
         <f aca="false">E39*B39</f>
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="G39" s="0"/>
       <c r="H39" s="0"/>
-      <c r="I39" s="11" t="s">
+      <c r="I39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="B40" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>565</v>
+        <v>105</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">E40*B40</f>
-        <v>565</v>
+        <v>0</v>
       </c>
       <c r="G40" s="0"/>
       <c r="H40" s="0"/>
-      <c r="I40" s="11" t="s">
+      <c r="I40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B41" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="0"/>
       <c r="E41" s="1" t="n">
-        <v>270</v>
+        <v>685</v>
       </c>
       <c r="F41" s="1" t="n">
         <f aca="false">E41*B41</f>
-        <v>270</v>
-      </c>
-      <c r="G41" s="12" t="n">
-        <v>40355</v>
-      </c>
+        <v>685</v>
+      </c>
+      <c r="G41" s="0"/>
       <c r="H41" s="0"/>
-      <c r="I41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>327.6</v>
+        <v>200</v>
       </c>
       <c r="F42" s="1" t="n">
         <f aca="false">E42*B42</f>
-        <v>327.6</v>
-      </c>
-      <c r="G42" s="12" t="n">
-        <v>40355</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="G42" s="0"/>
       <c r="H42" s="0"/>
-      <c r="I42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I42" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>203.69</v>
+        <v>565</v>
       </c>
       <c r="F43" s="1" t="n">
         <f aca="false">E43*B43</f>
-        <v>1222.14</v>
-      </c>
-      <c r="G43" s="12" t="n">
-        <v>40355</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="0"/>
+        <v>565</v>
+      </c>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D44" s="0"/>
       <c r="E44" s="1" t="n">
-        <v>103.01</v>
+        <v>270</v>
       </c>
       <c r="F44" s="1" t="n">
         <f aca="false">E44*B44</f>
-        <v>206.02</v>
-      </c>
-      <c r="G44" s="0"/>
-      <c r="H44" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G44" s="12" t="n">
+        <v>40355</v>
+      </c>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
+      <c r="D45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>327.6</v>
+      </c>
       <c r="F45" s="1" t="n">
         <f aca="false">E45*B45</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="0"/>
+        <v>327.6</v>
+      </c>
+      <c r="G45" s="12" t="n">
+        <v>40355</v>
+      </c>
+      <c r="H45" s="0"/>
       <c r="I45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
-      <c r="E46" s="0"/>
+      <c r="A46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>203.69</v>
+      </c>
       <c r="F46" s="1" t="n">
         <f aca="false">E46*B46</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="15"/>
+        <v>1222.14</v>
+      </c>
+      <c r="G46" s="12" t="n">
+        <v>40355</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="I46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="0"/>
-      <c r="D47" s="0"/>
-      <c r="E47" s="0"/>
+      <c r="A47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>103.01</v>
+      </c>
       <c r="F47" s="1" t="n">
         <f aca="false">E47*B47</f>
-        <v>0</v>
+        <v>206.02</v>
       </c>
       <c r="G47" s="0"/>
+      <c r="H47" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="I47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,73 +1820,93 @@
       <c r="I48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E49" s="1" t="n">
-        <v>285</v>
-      </c>
+      <c r="A49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
       <c r="F49" s="1" t="n">
         <f aca="false">E49*B49</f>
         <v>0</v>
       </c>
-      <c r="G49" s="12" t="n">
-        <v>39646</v>
-      </c>
+      <c r="G49" s="15"/>
       <c r="I49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E50" s="1" t="n">
-        <v>171.6</v>
-      </c>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
       <c r="F50" s="1" t="n">
         <f aca="false">E50*B50</f>
         <v>0</v>
       </c>
-      <c r="G50" s="12" t="n">
-        <v>40355</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>127</v>
-      </c>
+      <c r="G50" s="0"/>
+      <c r="I50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
       <c r="F51" s="1" t="n">
         <f aca="false">E51*B51</f>
         <v>0</v>
       </c>
+      <c r="G51" s="0"/>
+      <c r="I51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>285</v>
+      </c>
       <c r="F52" s="1" t="n">
         <f aca="false">E52*B52</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="12" t="n">
+        <v>39646</v>
+      </c>
+      <c r="I52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>171.6</v>
+      </c>
       <c r="F53" s="1" t="n">
         <f aca="false">E53*B53</f>
         <v>0</v>
+      </c>
+      <c r="G53" s="12" t="n">
+        <v>40355</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,6 +1942,24 @@
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F59" s="1" t="n">
         <f aca="false">E59*B59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F60" s="1" t="n">
+        <f aca="false">E60*B60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F61" s="1" t="n">
+        <f aca="false">E61*B61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="1" t="n">
+        <f aca="false">E62*B62</f>
         <v>0</v>
       </c>
     </row>
@@ -1894,10 +1979,11 @@
     <hyperlink ref="I30" r:id="rId12" display="http://www.californiapc.com"/>
     <hyperlink ref="I31" r:id="rId13" display="http://www.omega.com/pptst/PX409_Series.html"/>
     <hyperlink ref="I32" r:id="rId14" display="http://www.omega.com/pptst/PS_SNUBBERS.html"/>
-    <hyperlink ref="I38" r:id="rId15" display="http://www.campbellsci.com/hmp155a"/>
-    <hyperlink ref="I39" r:id="rId16" display="http://www.campbellsci.com/h41005-5"/>
-    <hyperlink ref="I40" r:id="rId17" display="http://www.campbellsci.com/ut10"/>
-    <hyperlink ref="I50" r:id="rId18" display="http://www.savillex.com/ProductDetail.aspx?ProductName=Coiled-tubing-PFA-116-ID-x-18-OD-100"/>
+    <hyperlink ref="I34" r:id="rId15" display="http://opto22.com/site/pr_details.aspx?cid=7&amp;item=ODC5"/>
+    <hyperlink ref="I41" r:id="rId16" display="http://www.campbellsci.com/hmp155a"/>
+    <hyperlink ref="I42" r:id="rId17" display="http://www.campbellsci.com/h41005-5"/>
+    <hyperlink ref="I43" r:id="rId18" display="http://www.campbellsci.com/ut10"/>
+    <hyperlink ref="I53" r:id="rId19" display="http://www.savillex.com/ProductDetail.aspx?ProductName=Coiled-tubing-PFA-116-ID-x-18-OD-100"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update price for MFC/relay enclosure
</commit_message>
<xml_diff>
--- a/doc/components.xlsx
+++ b/doc/components.xlsx
@@ -104,10 +104,10 @@
     <t>NL115-ST-SW</t>
   </si>
   <si>
-    <t>http://www.campbellsci.com/nl115 </t>
-  </si>
-  <si>
-    <t>Datalogger charger: 12-&gt;24V </t>
+    <t>http://www.campbellsci.com/nl115</t>
+  </si>
+  <si>
+    <t>Datalogger charger: 12-&gt;24V</t>
   </si>
   <si>
     <t>Digikey (CUI Inc)</t>
@@ -308,7 +308,7 @@
     <t>For valve control</t>
   </si>
   <si>
-    <t>http://opto22.com/site/pr_details.aspx?cid=7&amp;item=ODC5 </t>
+    <t>http://opto22.com/site/pr_details.aspx?cid=7&amp;item=ODC5</t>
   </si>
   <si>
     <t>Relay mounting board</t>
@@ -435,7 +435,7 @@
     <numFmt numFmtId="166" formatCode="_(\$* #,##0_);_(\$* \(#,##0\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -456,20 +456,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF800000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF008000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -493,24 +479,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99CC"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -528,7 +502,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -554,34 +528,28 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -589,56 +557,46 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Bad" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="22" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
@@ -647,15 +605,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+      <selection pane="bottomLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -696,7 +654,7 @@
       </c>
       <c r="F2" s="7" t="n">
         <f aca="false">SUM(F5:F1004)</f>
-        <v>19617.58</v>
+        <v>19689.57</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="0"/>
@@ -1006,10 +964,12 @@
       <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="0"/>
+      <c r="E15" s="1" t="n">
+        <v>39.99</v>
+      </c>
       <c r="F15" s="1" t="n">
         <f aca="false">E15*B15</f>
-        <v>0</v>
+        <v>39.99</v>
       </c>
       <c r="G15" s="12" t="n">
         <v>40355</v>
@@ -1446,7 +1406,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B33" s="2" t="n">
@@ -1470,7 +1430,7 @@
       <c r="I33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="2" t="n">
@@ -1484,6 +1444,10 @@
       </c>
       <c r="E34" s="1" t="n">
         <v>16</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <f aca="false">E34*B34</f>
+        <v>32</v>
       </c>
       <c r="G34" s="12" t="n">
         <v>40358</v>
@@ -1531,6 +1495,7 @@
       <c r="C36" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="D36" s="0"/>
       <c r="E36" s="1" t="n">
         <v>0</v>
       </c>
@@ -1553,11 +1518,19 @@
       <c r="B37" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="1" t="n">
+        <f aca="false">E37*B37</f>
+        <v>0</v>
+      </c>
       <c r="G37" s="12"/>
+      <c r="H37" s="0"/>
       <c r="I37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B38" s="2" t="n">
@@ -1616,6 +1589,8 @@
       <c r="C40" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
       <c r="F40" s="1" t="n">
         <f aca="false">E40*B40</f>
         <v>0</v>
@@ -1819,8 +1794,9 @@
       <c r="G48" s="0"/>
       <c r="I48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
       <c r="C49" s="0"/>
       <c r="D49" s="0"/>
       <c r="E49" s="0"/>
@@ -1828,7 +1804,6 @@
         <f aca="false">E49*B49</f>
         <v>0</v>
       </c>
-      <c r="G49" s="15"/>
       <c r="I49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,7 +1944,7 @@
     <hyperlink ref="I7" r:id="rId2" display="http://www.labcommerce.com/airsamp_viewproducts.php?catid=17"/>
     <hyperlink ref="I8" r:id="rId3" display="http://www.okcc.com/catsub_precision.htm"/>
     <hyperlink ref="I9" r:id="rId4" display="http://www.campbellsci.com/cr3000"/>
-    <hyperlink ref="I10" r:id="rId5" display="http://www.campbellsci.com/nl115 "/>
+    <hyperlink ref="I10" r:id="rId5" display="http://www.campbellsci.com/nl115"/>
     <hyperlink ref="I13" r:id="rId6" display="http://www.homedepot.com/p/Rubbermaid-Rattan-Patio-Cabinet-1863391/204725829?N=5yc1vZbtz1"/>
     <hyperlink ref="I14" r:id="rId7" display="http://www.campbellsci.com/enc-12-14-overview"/>
     <hyperlink ref="I15" r:id="rId8" display="http://www.walmart.com/ip/Plano-Guide-Series-PolyCarbonate-Box-Large-Blue/20563433"/>

</xml_diff>